<commit_message>
1. Merge conflict changes 2. Final changes
</commit_message>
<xml_diff>
--- a/TestSample.xlsx
+++ b/TestSample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="1712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="1708">
   <si>
     <t xml:space="preserve">rh</t>
   </si>
@@ -56,18 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">Country===3:::Maps===4:::1Up Travel - Maps of all the S - Category Countries of the world.===1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date:::Race:::Track:::Miles:::Type:::Winner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[[4/13/80, Datsun Twin 200, Ontario, 200, PO, Johnny Rutherford], [5/26/80, Indianapolis 500-Mile Race, Indianapolis, 500, PO, Johnny Rutherford], [6/8/80, Gould Rex Mays Classic, Milwaukee, 150, PO, Bobby Unser], [6/22/80, True Value 500, Pocono, 500, PO, Bobby Unser], [7/13/80, Red Roof Inns 150, Mid-Ohio, 156, RC, Johnny Rutherford], [7/20/80, Norton 200, MIS, 200, PO, Johnny Rutherford], [8/3/80, Kent Oil 150, Watkins Glen, 150.536, RC, Bobby Unser], [8/10/80, Tony Bettenhausen 200, Milwaukee, 200, PO, Johnny Rutherford], [8/31/80, California 500, Ontario, 500, PO, Bobby Unser], [9/20/80, Gould Grand Prix, MIS, 150, PO, Mario Andretti], [10/26/80, Primera Copa Mxico 150, Mexico City, 148.8, RC, Rick Mears], [11/8/80, Miller High Life 150, Phoenix, 150, PO, Tom Sneva]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1980 PPG Indy Car World Series</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1980 PPG Indy Car World Series===1:::Standing===4:::===3</t>
   </si>
   <si>
     <t xml:space="preserve">#:::Horse:::On-course prices:::Tote win:::Tote pl.:::SP</t>
@@ -5170,6 +5158,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -5255,10 +5244,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D450"/>
+  <dimension ref="A1:D449"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A446" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B450" activeCellId="0" sqref="B450"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5266,7 +5255,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="91.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="105.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="102.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="130.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="130.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -5312,7 +5301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -5326,7 +5315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="552.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>16</v>
       </c>
@@ -5340,7 +5329,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="552.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>20</v>
       </c>
@@ -5354,7 +5343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>24</v>
       </c>
@@ -5368,7 +5357,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>28</v>
       </c>
@@ -5382,7 +5371,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>32</v>
       </c>
@@ -5396,7 +5385,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="1442.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>36</v>
       </c>
@@ -5410,7 +5399,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="1442.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>40</v>
       </c>
@@ -5424,7 +5413,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="350.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>44</v>
       </c>
@@ -5438,7 +5427,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="350.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>48</v>
       </c>
@@ -5452,7 +5441,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="440.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>52</v>
       </c>
@@ -5466,7 +5455,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="440.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>56</v>
       </c>
@@ -5480,7 +5469,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>60</v>
       </c>
@@ -5494,7 +5483,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>64</v>
       </c>
@@ -5522,7 +5511,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>72</v>
       </c>
@@ -5536,7 +5525,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>76</v>
       </c>
@@ -5550,7 +5539,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>80</v>
       </c>
@@ -5564,7 +5553,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>84</v>
       </c>
@@ -5578,7 +5567,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="159" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>88</v>
       </c>
@@ -5592,7 +5581,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="159" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>92</v>
       </c>
@@ -5606,7 +5595,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>96</v>
       </c>
@@ -5620,7 +5609,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>100</v>
       </c>
@@ -5634,7 +5623,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>104</v>
       </c>
@@ -5648,7 +5637,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>108</v>
       </c>
@@ -5662,7 +5651,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>112</v>
       </c>
@@ -5676,7 +5665,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>116</v>
       </c>
@@ -5690,7 +5679,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="1509.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>120</v>
       </c>
@@ -5704,7 +5693,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="1509.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>124</v>
       </c>
@@ -5732,7 +5721,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>132</v>
       </c>
@@ -5746,7 +5735,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>136</v>
       </c>
@@ -5774,7 +5763,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>144</v>
       </c>
@@ -5788,7 +5777,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>148</v>
       </c>
@@ -5802,35 +5791,35 @@
         <v>151</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C39" s="1" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>158</v>
       </c>
@@ -5844,7 +5833,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>162</v>
       </c>
@@ -5858,7 +5847,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>166</v>
       </c>
@@ -5872,7 +5861,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="901.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>170</v>
       </c>
@@ -5886,7 +5875,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="901.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="474" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>174</v>
       </c>
@@ -5900,7 +5889,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="474" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>178</v>
       </c>
@@ -5914,7 +5903,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="845.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>182</v>
       </c>
@@ -5928,7 +5917,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="845.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>186</v>
       </c>
@@ -5942,7 +5931,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>190</v>
       </c>
@@ -5970,7 +5959,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>198</v>
       </c>
@@ -5984,7 +5973,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>202</v>
       </c>
@@ -5998,7 +5987,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="372.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>206</v>
       </c>
@@ -6012,7 +6001,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="372.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="507.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>210</v>
       </c>
@@ -6026,7 +6015,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="507.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>214</v>
       </c>
@@ -6040,23 +6029,23 @@
         <v>217</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="1059" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="D56" s="0" t="s">
+    </row>
+    <row r="57" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="1059" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>174</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>222</v>
@@ -6068,7 +6057,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>225</v>
       </c>
@@ -6082,7 +6071,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>229</v>
       </c>
@@ -6096,7 +6085,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>233</v>
       </c>
@@ -6110,7 +6099,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>237</v>
       </c>
@@ -6124,7 +6113,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>241</v>
       </c>
@@ -6138,7 +6127,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>245</v>
       </c>
@@ -6152,7 +6141,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>249</v>
       </c>
@@ -6166,7 +6155,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>253</v>
       </c>
@@ -6180,7 +6169,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>257</v>
       </c>
@@ -6194,7 +6183,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>261</v>
       </c>
@@ -6208,7 +6197,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>265</v>
       </c>
@@ -6222,7 +6211,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>269</v>
       </c>
@@ -6238,24 +6227,24 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="D70" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="C70" s="1" t="s">
+    </row>
+    <row r="71" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="B71" s="1" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>277</v>
@@ -6264,7 +6253,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>279</v>
       </c>
@@ -6278,7 +6267,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="609" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>283</v>
       </c>
@@ -6292,7 +6281,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="609" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>287</v>
       </c>
@@ -6306,7 +6295,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>291</v>
       </c>
@@ -6320,7 +6309,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="980.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>295</v>
       </c>
@@ -6334,7 +6323,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="980.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>299</v>
       </c>
@@ -6348,7 +6337,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>303</v>
       </c>
@@ -6362,7 +6351,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>307</v>
       </c>
@@ -6376,7 +6365,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="811.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>311</v>
       </c>
@@ -6390,7 +6379,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="811.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="1374.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>315</v>
       </c>
@@ -6404,7 +6393,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="1374.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>319</v>
       </c>
@@ -6432,7 +6421,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="282.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>327</v>
       </c>
@@ -6446,7 +6435,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="282.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>331</v>
       </c>
@@ -6460,7 +6449,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>335</v>
       </c>
@@ -6474,7 +6463,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>339</v>
       </c>
@@ -6488,7 +6477,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>343</v>
       </c>
@@ -6502,7 +6491,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>347</v>
       </c>
@@ -6516,23 +6505,23 @@
         <v>350</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="946.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="D90" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="D90" s="0" t="s">
+    </row>
+    <row r="91" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
         <v>354</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="946.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
-        <v>299</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>355</v>
@@ -6544,7 +6533,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>358</v>
       </c>
@@ -6558,7 +6547,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>362</v>
       </c>
@@ -6572,7 +6561,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>366</v>
       </c>
@@ -6586,7 +6575,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>370</v>
       </c>
@@ -6600,7 +6589,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>374</v>
       </c>
@@ -6614,7 +6603,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>378</v>
       </c>
@@ -6628,7 +6617,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>382</v>
       </c>
@@ -6642,7 +6631,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>386</v>
       </c>
@@ -6670,7 +6659,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>394</v>
       </c>
@@ -6684,7 +6673,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>398</v>
       </c>
@@ -6698,23 +6687,23 @@
         <v>401</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="C103" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="D103" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="D103" s="0" t="s">
+    </row>
+    <row r="104" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
         <v>405</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>406</v>
@@ -6726,7 +6715,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="519" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>409</v>
       </c>
@@ -6740,7 +6729,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="519" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>413</v>
       </c>
@@ -6754,7 +6743,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="552.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>417</v>
       </c>
@@ -6768,7 +6757,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="552.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>421</v>
       </c>
@@ -6782,7 +6771,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="417.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>425</v>
       </c>
@@ -6796,7 +6785,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="417.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="1656" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>429</v>
       </c>
@@ -6810,7 +6799,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="1656" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="372.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>433</v>
       </c>
@@ -6824,7 +6813,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="372.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>437</v>
       </c>
@@ -6838,23 +6827,23 @@
         <v>440</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="845.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="C113" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="D113" s="0" t="s">
         <v>443</v>
       </c>
-      <c r="D113" s="0" t="s">
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="845.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
-        <v>174</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>445</v>
@@ -6866,23 +6855,23 @@
         <v>447</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="D115" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="D115" s="0" t="s">
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
         <v>451</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>452</v>
@@ -6894,7 +6883,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>455</v>
       </c>
@@ -6908,7 +6897,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>459</v>
       </c>
@@ -6922,7 +6911,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>463</v>
       </c>
@@ -6936,7 +6925,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="755.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>467</v>
       </c>
@@ -6950,7 +6939,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="755.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="1689.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>471</v>
       </c>
@@ -6964,7 +6953,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="1689.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>475</v>
       </c>
@@ -6978,7 +6967,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>479</v>
       </c>
@@ -7006,7 +6995,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>487</v>
       </c>
@@ -7020,7 +7009,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>491</v>
       </c>
@@ -7034,7 +7023,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>495</v>
       </c>
@@ -7048,7 +7037,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>499</v>
       </c>
@@ -7062,7 +7051,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>503</v>
       </c>
@@ -7076,7 +7065,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>507</v>
       </c>
@@ -7090,7 +7079,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>511</v>
       </c>
@@ -7104,23 +7093,23 @@
         <v>514</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="C132" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="0" t="s">
         <v>517</v>
       </c>
-      <c r="D132" s="0" t="s">
+    </row>
+    <row r="133" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
         <v>518</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>214</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>519</v>
@@ -7132,7 +7121,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>522</v>
       </c>
@@ -7160,7 +7149,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>530</v>
       </c>
@@ -7174,7 +7163,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>534</v>
       </c>
@@ -7188,7 +7177,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="676.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>538</v>
       </c>
@@ -7202,7 +7191,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="676.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>542</v>
       </c>
@@ -7216,7 +7205,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="440.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>546</v>
       </c>
@@ -7230,7 +7219,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="440.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>550</v>
       </c>
@@ -7244,7 +7233,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>554</v>
       </c>
@@ -7258,7 +7247,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>558</v>
       </c>
@@ -7272,7 +7261,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>562</v>
       </c>
@@ -7286,7 +7275,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="159" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>566</v>
       </c>
@@ -7300,7 +7289,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="159" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>570</v>
       </c>
@@ -7314,7 +7303,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>574</v>
       </c>
@@ -7342,7 +7331,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>582</v>
       </c>
@@ -7356,7 +7345,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>586</v>
       </c>
@@ -7370,7 +7359,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="327.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>590</v>
       </c>
@@ -7384,7 +7373,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="327.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="1014" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>594</v>
       </c>
@@ -7398,7 +7387,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="1014" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>598</v>
       </c>
@@ -7412,7 +7401,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>602</v>
       </c>
@@ -7440,7 +7429,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>610</v>
       </c>
@@ -7454,7 +7443,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="462.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>614</v>
       </c>
@@ -7468,7 +7457,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="462.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="1137.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>618</v>
       </c>
@@ -7482,7 +7471,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="1137.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>622</v>
       </c>
@@ -7496,7 +7485,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>626</v>
       </c>
@@ -7524,7 +7513,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>634</v>
       </c>
@@ -7552,7 +7541,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>642</v>
       </c>
@@ -7566,7 +7555,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>646</v>
       </c>
@@ -7580,7 +7569,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="429" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>650</v>
       </c>
@@ -7594,26 +7583,26 @@
         <v>653</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="429" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C167" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="D167" s="0" t="s">
         <v>655</v>
       </c>
-      <c r="C167" s="1" t="s">
+    </row>
+    <row r="168" customFormat="false" ht="519" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
         <v>656</v>
       </c>
-      <c r="D167" s="0" t="s">
+      <c r="B168" s="1" t="s">
         <v>657</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>658</v>
@@ -7622,7 +7611,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="519" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>660</v>
       </c>
@@ -7636,7 +7625,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>664</v>
       </c>
@@ -7650,7 +7639,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>668</v>
       </c>
@@ -7664,7 +7653,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="721.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>672</v>
       </c>
@@ -7678,7 +7667,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="721.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>676</v>
       </c>
@@ -7692,7 +7681,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="912.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>680</v>
       </c>
@@ -7706,7 +7695,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="912.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>684</v>
       </c>
@@ -7720,7 +7709,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>688</v>
       </c>
@@ -7734,7 +7723,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>692</v>
       </c>
@@ -7748,7 +7737,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="339" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>696</v>
       </c>
@@ -7762,7 +7751,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="339" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>700</v>
       </c>
@@ -7776,7 +7765,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>704</v>
       </c>
@@ -7790,7 +7779,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>708</v>
       </c>
@@ -7804,7 +7793,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>712</v>
       </c>
@@ -7818,7 +7807,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
         <v>716</v>
       </c>
@@ -7832,7 +7821,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
         <v>720</v>
       </c>
@@ -7846,7 +7835,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>724</v>
       </c>
@@ -7860,7 +7849,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>728</v>
       </c>
@@ -7874,23 +7863,23 @@
         <v>731</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="C187" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="C187" s="1" t="s">
+      <c r="D187" s="0" t="s">
         <v>734</v>
       </c>
-      <c r="D187" s="0" t="s">
+    </row>
+    <row r="188" customFormat="false" ht="620.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
         <v>735</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
-        <v>390</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>736</v>
@@ -7902,7 +7891,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="620.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
         <v>739</v>
       </c>
@@ -7916,7 +7905,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
         <v>743</v>
       </c>
@@ -7930,7 +7919,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
         <v>747</v>
       </c>
@@ -7944,7 +7933,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
         <v>751</v>
       </c>
@@ -7958,7 +7947,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
         <v>755</v>
       </c>
@@ -7972,7 +7961,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="451.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>759</v>
       </c>
@@ -7986,7 +7975,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="451.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>763</v>
       </c>
@@ -8000,7 +7989,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>767</v>
       </c>
@@ -8014,7 +8003,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
         <v>771</v>
       </c>
@@ -8028,7 +8017,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="1296" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
         <v>775</v>
       </c>
@@ -8042,7 +8031,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="1296" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="642.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>779</v>
       </c>
@@ -8056,7 +8045,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="642.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>783</v>
       </c>
@@ -8070,7 +8059,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>787</v>
       </c>
@@ -8084,7 +8073,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
         <v>791</v>
       </c>
@@ -8098,7 +8087,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
         <v>795</v>
       </c>
@@ -8112,7 +8101,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="204" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
         <v>799</v>
       </c>
@@ -8126,7 +8115,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
         <v>803</v>
       </c>
@@ -8154,7 +8143,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
         <v>811</v>
       </c>
@@ -8168,7 +8157,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="208" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" customFormat="false" ht="541.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
         <v>815</v>
       </c>
@@ -8182,7 +8171,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="541.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
         <v>819</v>
       </c>
@@ -8196,7 +8185,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="210" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
         <v>823</v>
       </c>
@@ -8210,7 +8199,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="211" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
         <v>827</v>
       </c>
@@ -8224,7 +8213,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="212" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
         <v>831</v>
       </c>
@@ -8238,7 +8227,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="213" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" customFormat="false" ht="350.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
         <v>835</v>
       </c>
@@ -8252,23 +8241,23 @@
         <v>838</v>
       </c>
     </row>
-    <row r="214" customFormat="false" ht="350.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" customFormat="false" ht="519" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="B214" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="C214" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="C214" s="1" t="s">
+      <c r="D214" s="0" t="s">
         <v>841</v>
       </c>
-      <c r="D214" s="0" t="s">
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
         <v>842</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="519" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
-        <v>660</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>843</v>
@@ -8294,7 +8283,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
         <v>850</v>
       </c>
@@ -8308,7 +8297,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="218" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
         <v>854</v>
       </c>
@@ -8322,7 +8311,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="219" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
         <v>858</v>
       </c>
@@ -8336,7 +8325,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="220" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
         <v>862</v>
       </c>
@@ -8350,7 +8339,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="221" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" customFormat="false" ht="1217.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
         <v>866</v>
       </c>
@@ -8364,7 +8353,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="222" customFormat="false" ht="1217.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
         <v>870</v>
       </c>
@@ -8378,37 +8367,37 @@
         <v>873</v>
       </c>
     </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" customFormat="false" ht="665.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="B223" s="1" t="s">
         <v>874</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="C223" s="1" t="s">
         <v>875</v>
       </c>
-      <c r="C223" s="1" t="s">
+      <c r="D223" s="0" t="s">
         <v>876</v>
       </c>
-      <c r="D223" s="0" t="s">
+    </row>
+    <row r="224" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>877</v>
       </c>
-    </row>
-    <row r="224" customFormat="false" ht="665.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="B224" s="1" t="s">
+      <c r="C224" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="C224" s="1" t="s">
+      <c r="D224" s="0" t="s">
         <v>879</v>
       </c>
-      <c r="D224" s="0" t="s">
+    </row>
+    <row r="225" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
         <v>880</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="0" t="s">
-        <v>831</v>
       </c>
       <c r="B225" s="1" t="s">
         <v>881</v>
@@ -8420,7 +8409,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="226" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" customFormat="false" ht="1892.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
         <v>884</v>
       </c>
@@ -8434,7 +8423,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="227" customFormat="false" ht="1892.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
         <v>888</v>
       </c>
@@ -8448,7 +8437,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="228" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="946.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
         <v>892</v>
       </c>
@@ -8462,7 +8451,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="229" customFormat="false" ht="946.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
         <v>896</v>
       </c>
@@ -8476,7 +8465,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" customFormat="false" ht="249" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
         <v>900</v>
       </c>
@@ -8490,7 +8479,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="231" customFormat="false" ht="249" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
         <v>904</v>
       </c>
@@ -8504,7 +8493,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
         <v>908</v>
       </c>
@@ -8518,7 +8507,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="233" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
         <v>912</v>
       </c>
@@ -8532,7 +8521,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="234" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" customFormat="false" ht="552.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
         <v>916</v>
       </c>
@@ -8546,7 +8535,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="552.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
         <v>920</v>
       </c>
@@ -8574,23 +8563,23 @@
         <v>927</v>
       </c>
     </row>
-    <row r="237" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B237" s="1" t="s">
         <v>928</v>
       </c>
-      <c r="B237" s="1" t="s">
+      <c r="C237" s="1" t="s">
         <v>929</v>
       </c>
-      <c r="C237" s="1" t="s">
+      <c r="D237" s="0" t="s">
         <v>930</v>
       </c>
-      <c r="D237" s="0" t="s">
+    </row>
+    <row r="238" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
         <v>931</v>
-      </c>
-    </row>
-    <row r="238" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="0" t="s">
-        <v>36</v>
       </c>
       <c r="B238" s="1" t="s">
         <v>932</v>
@@ -8602,7 +8591,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="239" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
         <v>935</v>
       </c>
@@ -8616,7 +8605,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
         <v>939</v>
       </c>
@@ -8630,7 +8619,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="1329.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
         <v>943</v>
       </c>
@@ -8644,7 +8633,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="242" customFormat="false" ht="1329.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
         <v>947</v>
       </c>
@@ -8658,7 +8647,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="243" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
         <v>951</v>
       </c>
@@ -8672,7 +8661,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="271.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="316.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
         <v>955</v>
       </c>
@@ -8686,7 +8675,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="245" customFormat="false" ht="316.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
         <v>959</v>
       </c>
@@ -8700,7 +8689,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
         <v>963</v>
       </c>
@@ -8714,7 +8703,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="247" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" customFormat="false" ht="1059" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
         <v>967</v>
       </c>
@@ -8728,7 +8717,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="248" customFormat="false" ht="1059" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
         <v>971</v>
       </c>
@@ -8742,23 +8731,23 @@
         <v>974</v>
       </c>
     </row>
-    <row r="249" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B249" s="1" t="s">
         <v>975</v>
       </c>
-      <c r="B249" s="1" t="s">
+      <c r="C249" s="1" t="s">
         <v>976</v>
       </c>
-      <c r="C249" s="1" t="s">
+      <c r="D249" s="0" t="s">
         <v>977</v>
       </c>
-      <c r="D249" s="0" t="s">
+    </row>
+    <row r="250" customFormat="false" ht="530.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
         <v>978</v>
-      </c>
-    </row>
-    <row r="250" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="0" t="s">
-        <v>225</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>979</v>
@@ -8770,7 +8759,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="251" customFormat="false" ht="530.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
         <v>982</v>
       </c>
@@ -8784,7 +8773,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="252" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" customFormat="false" ht="879" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
         <v>986</v>
       </c>
@@ -8798,7 +8787,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="253" customFormat="false" ht="879" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" customFormat="false" ht="2252.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
         <v>990</v>
       </c>
@@ -8812,23 +8801,23 @@
         <v>993</v>
       </c>
     </row>
-    <row r="254" customFormat="false" ht="2252.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
+        <v>924</v>
+      </c>
+      <c r="B254" s="1" t="s">
         <v>994</v>
       </c>
-      <c r="B254" s="1" t="s">
+      <c r="C254" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="C254" s="1" t="s">
+      <c r="D254" s="0" t="s">
         <v>996</v>
       </c>
-      <c r="D254" s="0" t="s">
+    </row>
+    <row r="255" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
         <v>997</v>
-      </c>
-    </row>
-    <row r="255" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="0" t="s">
-        <v>928</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>998</v>
@@ -8840,23 +8829,23 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="256" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B256" s="1" t="s">
         <v>1001</v>
       </c>
-      <c r="B256" s="1" t="s">
+      <c r="C256" s="1" t="s">
         <v>1002</v>
       </c>
-      <c r="C256" s="1" t="s">
+      <c r="D256" s="0" t="s">
         <v>1003</v>
       </c>
-      <c r="D256" s="0" t="s">
+    </row>
+    <row r="257" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
         <v>1004</v>
-      </c>
-    </row>
-    <row r="257" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="0" t="s">
-        <v>68</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>1005</v>
@@ -8868,35 +8857,35 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="258" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" customFormat="false" ht="327.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="B258" s="1" t="s">
         <v>1008</v>
       </c>
-      <c r="B258" s="1" t="s">
+      <c r="C258" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D258" s="0" t="s">
         <v>1009</v>
       </c>
-      <c r="C258" s="1" t="s">
+    </row>
+    <row r="259" customFormat="false" ht="1757.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
         <v>1010</v>
       </c>
-      <c r="D258" s="0" t="s">
+      <c r="B259" s="1" t="s">
         <v>1011</v>
       </c>
-    </row>
-    <row r="259" customFormat="false" ht="327.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B259" s="1" t="s">
+      <c r="C259" s="1" t="s">
         <v>1012</v>
-      </c>
-      <c r="C259" s="1" t="s">
-        <v>914</v>
       </c>
       <c r="D259" s="0" t="s">
         <v>1013</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="1757.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" customFormat="false" ht="417.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
         <v>1014</v>
       </c>
@@ -8910,7 +8899,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="261" customFormat="false" ht="417.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
         <v>1018</v>
       </c>
@@ -8924,7 +8913,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="262" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
         <v>1022</v>
       </c>
@@ -8938,7 +8927,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="263" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
         <v>1026</v>
       </c>
@@ -8952,23 +8941,23 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="264" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" customFormat="false" ht="1025.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B264" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="B264" s="1" t="s">
+      <c r="C264" s="1" t="s">
         <v>1031</v>
       </c>
-      <c r="C264" s="1" t="s">
+      <c r="D264" s="0" t="s">
         <v>1032</v>
       </c>
-      <c r="D264" s="0" t="s">
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
         <v>1033</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="1025.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="0" t="s">
-        <v>174</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>1034</v>
@@ -8980,7 +8969,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
         <v>1037</v>
       </c>
@@ -8994,7 +8983,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" customFormat="false" ht="417.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
         <v>1041</v>
       </c>
@@ -9008,7 +8997,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="268" customFormat="false" ht="417.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
         <v>1045</v>
       </c>
@@ -9022,7 +9011,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="269" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" customFormat="false" ht="822.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
         <v>1049</v>
       </c>
@@ -9036,23 +9025,23 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="270" customFormat="false" ht="822.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" customFormat="false" ht="620.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B270" s="1" t="s">
         <v>1053</v>
       </c>
-      <c r="B270" s="1" t="s">
+      <c r="C270" s="1" t="s">
         <v>1054</v>
       </c>
-      <c r="C270" s="1" t="s">
+      <c r="D270" s="0" t="s">
         <v>1055</v>
       </c>
-      <c r="D270" s="0" t="s">
+    </row>
+    <row r="271" customFormat="false" ht="1296" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
         <v>1056</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="620.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="0" t="s">
-        <v>174</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>1057</v>
@@ -9064,7 +9053,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="272" customFormat="false" ht="1296" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
         <v>1060</v>
       </c>
@@ -9078,7 +9067,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="273" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" customFormat="false" ht="1036.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
         <v>1064</v>
       </c>
@@ -9092,7 +9081,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="274" customFormat="false" ht="1036.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
         <v>1068</v>
       </c>
@@ -9106,7 +9095,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="275" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
         <v>1072</v>
       </c>
@@ -9120,23 +9109,23 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="276" customFormat="false" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B276" s="1" t="s">
         <v>1076</v>
       </c>
-      <c r="B276" s="1" t="s">
+      <c r="C276" s="1" t="s">
         <v>1077</v>
       </c>
-      <c r="C276" s="1" t="s">
+      <c r="D276" s="0" t="s">
         <v>1078</v>
       </c>
-      <c r="D276" s="0" t="s">
+    </row>
+    <row r="277" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
         <v>1079</v>
-      </c>
-    </row>
-    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="B277" s="1" t="s">
         <v>1080</v>
@@ -9148,23 +9137,23 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="278" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" customFormat="false" ht="1002.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B278" s="1" t="s">
         <v>1083</v>
       </c>
-      <c r="B278" s="1" t="s">
+      <c r="C278" s="1" t="s">
         <v>1084</v>
       </c>
-      <c r="C278" s="1" t="s">
+      <c r="D278" s="0" t="s">
         <v>1085</v>
       </c>
-      <c r="D278" s="0" t="s">
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="s">
         <v>1086</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="1002.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="0" t="s">
-        <v>174</v>
       </c>
       <c r="B279" s="1" t="s">
         <v>1087</v>
@@ -9176,7 +9165,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
         <v>1090</v>
       </c>
@@ -9190,49 +9179,49 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="281" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
+        <v>642</v>
+      </c>
+      <c r="B281" s="1" t="s">
         <v>1094</v>
       </c>
-      <c r="B281" s="1" t="s">
+      <c r="C281" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D281" s="0" t="s">
         <v>1095</v>
       </c>
-      <c r="C281" s="1" t="s">
+    </row>
+    <row r="282" customFormat="false" ht="327.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="D282" s="0" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
         <v>1096</v>
       </c>
-      <c r="D281" s="0" t="s">
+      <c r="B283" s="1" t="s">
         <v>1097</v>
       </c>
-    </row>
-    <row r="282" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="0" t="s">
-        <v>646</v>
-      </c>
-      <c r="B282" s="1" t="s">
+      <c r="C283" s="1" t="s">
         <v>1098</v>
       </c>
-      <c r="C282" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D282" s="0" t="s">
+      <c r="D283" s="0" t="s">
         <v>1099</v>
       </c>
     </row>
-    <row r="283" customFormat="false" ht="327.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="0" t="s">
-        <v>594</v>
-      </c>
-      <c r="B283" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="C283" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="D283" s="0" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="284" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
         <v>1100</v>
       </c>
@@ -9246,7 +9235,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="285" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" customFormat="false" ht="316.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
         <v>1104</v>
       </c>
@@ -9260,7 +9249,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="316.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
         <v>1108</v>
       </c>
@@ -9274,7 +9263,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="287" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
         <v>1112</v>
       </c>
@@ -9288,7 +9277,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="288" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="0" t="s">
         <v>1116</v>
       </c>
@@ -9302,7 +9291,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="289" customFormat="false" ht="237.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
         <v>1120</v>
       </c>
@@ -9316,35 +9305,35 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="290" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
+        <v>534</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D290" s="0" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="0" t="s">
         <v>1124</v>
       </c>
-      <c r="B290" s="1" t="s">
+      <c r="B291" s="1" t="s">
         <v>1125</v>
       </c>
-      <c r="C290" s="1" t="s">
+      <c r="C291" s="1" t="s">
         <v>1126</v>
       </c>
-      <c r="D290" s="0" t="s">
+      <c r="D291" s="0" t="s">
         <v>1127</v>
       </c>
     </row>
-    <row r="291" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="0" t="s">
-        <v>538</v>
-      </c>
-      <c r="B291" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="C291" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="D291" s="0" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
         <v>1128</v>
       </c>
@@ -9358,35 +9347,35 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="B293" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="B293" s="1" t="s">
+      <c r="C293" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D293" s="0" t="s">
         <v>1133</v>
       </c>
-      <c r="C293" s="1" t="s">
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
         <v>1134</v>
       </c>
-      <c r="D293" s="0" t="s">
+      <c r="B294" s="1" t="s">
         <v>1135</v>
       </c>
-    </row>
-    <row r="294" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B294" s="1" t="s">
+      <c r="C294" s="1" t="s">
         <v>1136</v>
-      </c>
-      <c r="C294" s="1" t="s">
-        <v>914</v>
       </c>
       <c r="D294" s="0" t="s">
         <v>1137</v>
       </c>
     </row>
-    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" customFormat="false" ht="789" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
         <v>1138</v>
       </c>
@@ -9400,23 +9389,23 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="296" customFormat="false" ht="789" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
+        <v>700</v>
+      </c>
+      <c r="B296" s="1" t="s">
         <v>1142</v>
       </c>
-      <c r="B296" s="1" t="s">
+      <c r="C296" s="1" t="s">
         <v>1143</v>
       </c>
-      <c r="C296" s="1" t="s">
+      <c r="D296" s="0" t="s">
         <v>1144</v>
       </c>
-      <c r="D296" s="0" t="s">
+    </row>
+    <row r="297" customFormat="false" ht="845.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A297" s="0" t="s">
         <v>1145</v>
-      </c>
-    </row>
-    <row r="297" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="0" t="s">
-        <v>704</v>
       </c>
       <c r="B297" s="1" t="s">
         <v>1146</v>
@@ -9428,7 +9417,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="298" customFormat="false" ht="845.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
         <v>1149</v>
       </c>
@@ -9442,7 +9431,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
         <v>1153</v>
       </c>
@@ -9456,7 +9445,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
         <v>1157</v>
       </c>
@@ -9470,7 +9459,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="301" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
         <v>1161</v>
       </c>
@@ -9484,7 +9473,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="302" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
         <v>1165</v>
       </c>
@@ -9498,7 +9487,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="303" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
         <v>1169</v>
       </c>
@@ -9526,7 +9515,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" customFormat="false" ht="957.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
         <v>1177</v>
       </c>
@@ -9540,7 +9529,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="306" customFormat="false" ht="957.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
         <v>1181</v>
       </c>
@@ -9568,7 +9557,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="0" t="s">
         <v>1189</v>
       </c>
@@ -9582,7 +9571,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" customFormat="false" ht="620.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
         <v>1193</v>
       </c>
@@ -9596,23 +9585,23 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="310" customFormat="false" ht="620.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" customFormat="false" ht="339" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B310" s="1" t="s">
         <v>1197</v>
       </c>
-      <c r="B310" s="1" t="s">
+      <c r="C310" s="1" t="s">
         <v>1198</v>
       </c>
-      <c r="C310" s="1" t="s">
+      <c r="D310" s="0" t="s">
         <v>1199</v>
       </c>
-      <c r="D310" s="0" t="s">
+    </row>
+    <row r="311" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="0" t="s">
         <v>1200</v>
-      </c>
-    </row>
-    <row r="311" customFormat="false" ht="339" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="B311" s="1" t="s">
         <v>1201</v>
@@ -9624,23 +9613,23 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="312" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B312" s="1" t="s">
         <v>1204</v>
       </c>
-      <c r="B312" s="1" t="s">
+      <c r="C312" s="1" t="s">
         <v>1205</v>
       </c>
-      <c r="C312" s="1" t="s">
+      <c r="D312" s="0" t="s">
         <v>1206</v>
       </c>
-      <c r="D312" s="0" t="s">
+    </row>
+    <row r="313" customFormat="false" ht="1307.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
         <v>1207</v>
-      </c>
-    </row>
-    <row r="313" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="0" t="s">
-        <v>1165</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>1208</v>
@@ -9652,35 +9641,35 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="314" customFormat="false" ht="1307.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B314" s="1" t="s">
         <v>1211</v>
       </c>
-      <c r="B314" s="1" t="s">
+      <c r="C314" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D314" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="710.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="s">
         <v>1212</v>
       </c>
-      <c r="C314" s="1" t="s">
+      <c r="B315" s="1" t="s">
         <v>1213</v>
       </c>
-      <c r="D314" s="0" t="s">
+      <c r="C315" s="1" t="s">
         <v>1214</v>
       </c>
-    </row>
-    <row r="315" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B315" s="1" t="s">
+      <c r="D315" s="0" t="s">
         <v>1215</v>
       </c>
-      <c r="C315" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D315" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="316" customFormat="false" ht="710.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="316" customFormat="false" ht="620.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="0" t="s">
         <v>1216</v>
       </c>
@@ -9694,7 +9683,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="317" customFormat="false" ht="620.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="0" t="s">
         <v>1220</v>
       </c>
@@ -9708,7 +9697,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="318" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="0" t="s">
         <v>1224</v>
       </c>
@@ -9722,7 +9711,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="0" t="s">
         <v>1228</v>
       </c>
@@ -9736,7 +9725,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="320" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="0" t="s">
         <v>1232</v>
       </c>
@@ -9750,7 +9739,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="321" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="0" t="s">
         <v>1236</v>
       </c>
@@ -9764,23 +9753,23 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="322" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" customFormat="false" ht="474" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="B322" s="1" t="s">
         <v>1240</v>
       </c>
-      <c r="B322" s="1" t="s">
+      <c r="C322" s="1" t="s">
         <v>1241</v>
       </c>
-      <c r="C322" s="1" t="s">
+      <c r="D322" s="0" t="s">
         <v>1242</v>
       </c>
-      <c r="D322" s="0" t="s">
+    </row>
+    <row r="323" customFormat="false" ht="744" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="s">
         <v>1243</v>
-      </c>
-    </row>
-    <row r="323" customFormat="false" ht="474" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="0" t="s">
-        <v>660</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>1244</v>
@@ -9792,7 +9781,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="324" customFormat="false" ht="744" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="0" t="s">
         <v>1247</v>
       </c>
@@ -9806,23 +9795,23 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="B325" s="1" t="s">
         <v>1251</v>
       </c>
-      <c r="B325" s="1" t="s">
+      <c r="C325" s="1" t="s">
         <v>1252</v>
       </c>
-      <c r="C325" s="1" t="s">
+      <c r="D325" s="0" t="s">
         <v>1253</v>
       </c>
-      <c r="D325" s="0" t="s">
+    </row>
+    <row r="326" customFormat="false" ht="1092.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A326" s="0" t="s">
         <v>1254</v>
-      </c>
-    </row>
-    <row r="326" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="0" t="s">
-        <v>831</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>1255</v>
@@ -9834,7 +9823,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="327" customFormat="false" ht="1092.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" customFormat="false" ht="1217.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="0" t="s">
         <v>1258</v>
       </c>
@@ -9848,7 +9837,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="328" customFormat="false" ht="1217.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" customFormat="false" ht="519" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="0" t="s">
         <v>1262</v>
       </c>
@@ -9862,7 +9851,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="329" customFormat="false" ht="519" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="0" t="s">
         <v>1266</v>
       </c>
@@ -9876,7 +9865,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="330" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="0" t="s">
         <v>1270</v>
       </c>
@@ -9890,23 +9879,23 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="331" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="0" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B331" s="1" t="s">
         <v>1274</v>
       </c>
-      <c r="B331" s="1" t="s">
+      <c r="C331" s="1" t="s">
         <v>1275</v>
       </c>
-      <c r="C331" s="1" t="s">
+      <c r="D331" s="0" t="s">
         <v>1276</v>
       </c>
-      <c r="D331" s="0" t="s">
+    </row>
+    <row r="332" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="s">
         <v>1277</v>
-      </c>
-    </row>
-    <row r="332" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="0" t="s">
-        <v>1072</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>1278</v>
@@ -9918,26 +9907,26 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="333" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="0" t="s">
+        <v>846</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C333" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="B333" s="1" t="s">
+      <c r="D333" s="0" t="s">
         <v>1282</v>
       </c>
-      <c r="C333" s="1" t="s">
+    </row>
+    <row r="334" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
         <v>1283</v>
       </c>
-      <c r="D333" s="0" t="s">
+      <c r="B334" s="1" t="s">
         <v>1284</v>
-      </c>
-    </row>
-    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="0" t="s">
-        <v>850</v>
-      </c>
-      <c r="B334" s="1" t="s">
-        <v>851</v>
       </c>
       <c r="C334" s="1" t="s">
         <v>1285</v>
@@ -9946,37 +9935,37 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="335" customFormat="false" ht="192.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B335" s="1" t="s">
         <v>1287</v>
       </c>
-      <c r="B335" s="1" t="s">
+      <c r="C335" s="1" t="s">
         <v>1288</v>
       </c>
-      <c r="C335" s="1" t="s">
+      <c r="D335" s="0" t="s">
         <v>1289</v>
       </c>
-      <c r="D335" s="0" t="s">
+    </row>
+    <row r="336" customFormat="false" ht="451.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="B336" s="1" t="s">
         <v>1290</v>
       </c>
-    </row>
-    <row r="336" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B336" s="1" t="s">
+      <c r="C336" s="1" t="s">
         <v>1291</v>
       </c>
-      <c r="C336" s="1" t="s">
+      <c r="D336" s="0" t="s">
         <v>1292</v>
       </c>
-      <c r="D336" s="0" t="s">
+    </row>
+    <row r="337" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
         <v>1293</v>
-      </c>
-    </row>
-    <row r="337" customFormat="false" ht="451.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="0" t="s">
-        <v>660</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>1294</v>
@@ -9988,35 +9977,35 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="B338" s="1" t="s">
         <v>1297</v>
       </c>
-      <c r="B338" s="1" t="s">
+      <c r="C338" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D338" s="0" t="s">
         <v>1298</v>
       </c>
-      <c r="C338" s="1" t="s">
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
         <v>1299</v>
       </c>
-      <c r="D338" s="0" t="s">
+      <c r="B339" s="1" t="s">
         <v>1300</v>
       </c>
-    </row>
-    <row r="339" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B339" s="1" t="s">
+      <c r="C339" s="1" t="s">
         <v>1301</v>
-      </c>
-      <c r="C339" s="1" t="s">
-        <v>914</v>
       </c>
       <c r="D339" s="0" t="s">
         <v>1302</v>
       </c>
     </row>
-    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" customFormat="false" ht="496.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="0" t="s">
         <v>1303</v>
       </c>
@@ -10030,40 +10019,40 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="341" customFormat="false" ht="496.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B341" s="1" t="s">
         <v>1307</v>
       </c>
-      <c r="B341" s="1" t="s">
+      <c r="C341" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D341" s="0" t="s">
         <v>1308</v>
       </c>
-      <c r="C341" s="1" t="s">
+    </row>
+    <row r="342" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="C342" s="1" t="s">
         <v>1309</v>
       </c>
-      <c r="D341" s="0" t="s">
+      <c r="D342" s="0" t="s">
         <v>1310</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="0" t="s">
-        <v>503</v>
-      </c>
-      <c r="B342" s="1" t="s">
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
         <v>1311</v>
       </c>
-      <c r="C342" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="D342" s="0" t="s">
+      <c r="B343" s="1" t="s">
         <v>1312</v>
-      </c>
-    </row>
-    <row r="343" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="0" t="s">
-        <v>672</v>
-      </c>
-      <c r="B343" s="1" t="s">
-        <v>673</v>
       </c>
       <c r="C343" s="1" t="s">
         <v>1313</v>
@@ -10072,7 +10061,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" customFormat="false" ht="485.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="0" t="s">
         <v>1315</v>
       </c>
@@ -10086,7 +10075,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="485.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="249" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="0" t="s">
         <v>1319</v>
       </c>
@@ -10100,7 +10089,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="346" customFormat="false" ht="249" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="0" t="s">
         <v>1323</v>
       </c>
@@ -10114,7 +10103,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="924" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="0" t="s">
         <v>1327</v>
       </c>
@@ -10128,7 +10117,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="924" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="0" t="s">
         <v>1331</v>
       </c>
@@ -10142,7 +10131,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="0" t="s">
         <v>1335</v>
       </c>
@@ -10156,23 +10145,23 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B350" s="1" t="s">
         <v>1339</v>
       </c>
-      <c r="B350" s="1" t="s">
+      <c r="C350" s="1" t="s">
         <v>1340</v>
       </c>
-      <c r="C350" s="1" t="s">
+      <c r="D350" s="0" t="s">
         <v>1341</v>
       </c>
-      <c r="D350" s="0" t="s">
+    </row>
+    <row r="351" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="s">
         <v>1342</v>
-      </c>
-    </row>
-    <row r="351" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>1343</v>
@@ -10184,7 +10173,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="147.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="0" t="s">
         <v>1346</v>
       </c>
@@ -10198,7 +10187,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="353" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="0" t="s">
         <v>1350</v>
       </c>
@@ -10212,7 +10201,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="354" customFormat="false" ht="361.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="0" t="s">
         <v>1354</v>
       </c>
@@ -10226,7 +10215,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="355" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="0" t="s">
         <v>1358</v>
       </c>
@@ -10240,23 +10229,23 @@
         <v>1361</v>
       </c>
     </row>
-    <row r="356" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" customFormat="false" ht="462.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="0" t="s">
+        <v>759</v>
+      </c>
+      <c r="B356" s="1" t="s">
         <v>1362</v>
       </c>
-      <c r="B356" s="1" t="s">
+      <c r="C356" s="1" t="s">
         <v>1363</v>
       </c>
-      <c r="C356" s="1" t="s">
+      <c r="D356" s="0" t="s">
         <v>1364</v>
-      </c>
-      <c r="D356" s="0" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="462.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="0" t="s">
-        <v>763</v>
+        <v>1365</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>1366</v>
@@ -10268,7 +10257,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="358" customFormat="false" ht="462.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="0" t="s">
         <v>1369</v>
       </c>
@@ -10282,26 +10271,26 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C359" s="1" t="s">
         <v>1373</v>
       </c>
-      <c r="B359" s="1" t="s">
+      <c r="D359" s="0" t="s">
         <v>1374</v>
       </c>
-      <c r="C359" s="1" t="s">
+    </row>
+    <row r="360" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
         <v>1375</v>
       </c>
-      <c r="D359" s="0" t="s">
+      <c r="B360" s="1" t="s">
         <v>1376</v>
-      </c>
-    </row>
-    <row r="360" customFormat="false" ht="181.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B360" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="C360" s="1" t="s">
         <v>1377</v>
@@ -10324,7 +10313,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="362" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" customFormat="false" ht="597.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="0" t="s">
         <v>1383</v>
       </c>
@@ -10338,7 +10327,7 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="363" customFormat="false" ht="597.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" customFormat="false" ht="1779.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="0" t="s">
         <v>1387</v>
       </c>
@@ -10352,7 +10341,7 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="1779.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" customFormat="false" ht="1622.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="0" t="s">
         <v>1391</v>
       </c>
@@ -10366,7 +10355,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="365" customFormat="false" ht="1622.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="0" t="s">
         <v>1395</v>
       </c>
@@ -10380,7 +10369,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="366" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" customFormat="false" ht="417.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="0" t="s">
         <v>1399</v>
       </c>
@@ -10394,7 +10383,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="367" customFormat="false" ht="417.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" customFormat="false" ht="1723.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="0" t="s">
         <v>1403</v>
       </c>
@@ -10408,7 +10397,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="368" customFormat="false" ht="1723.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="0" t="s">
         <v>1407</v>
       </c>
@@ -10422,7 +10411,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="369" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="0" t="s">
         <v>1411</v>
       </c>
@@ -10436,7 +10425,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="0" t="s">
         <v>1415</v>
       </c>
@@ -10450,23 +10439,23 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="371" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" customFormat="false" ht="1070.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B371" s="1" t="s">
         <v>1419</v>
       </c>
-      <c r="B371" s="1" t="s">
+      <c r="C371" s="1" t="s">
         <v>1420</v>
       </c>
-      <c r="C371" s="1" t="s">
+      <c r="D371" s="0" t="s">
         <v>1421</v>
       </c>
-      <c r="D371" s="0" t="s">
+    </row>
+    <row r="372" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A372" s="0" t="s">
         <v>1422</v>
-      </c>
-    </row>
-    <row r="372" customFormat="false" ht="1070.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="0" t="s">
-        <v>1232</v>
       </c>
       <c r="B372" s="1" t="s">
         <v>1423</v>
@@ -10478,23 +10467,23 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="373" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="373" customFormat="false" ht="474" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B373" s="1" t="s">
         <v>1426</v>
       </c>
-      <c r="B373" s="1" t="s">
+      <c r="C373" s="1" t="s">
         <v>1427</v>
       </c>
-      <c r="C373" s="1" t="s">
+      <c r="D373" s="0" t="s">
         <v>1428</v>
       </c>
-      <c r="D373" s="0" t="s">
+    </row>
+    <row r="374" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="0" t="s">
         <v>1429</v>
-      </c>
-    </row>
-    <row r="374" customFormat="false" ht="474" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="0" t="s">
-        <v>390</v>
       </c>
       <c r="B374" s="1" t="s">
         <v>1430</v>
@@ -10506,7 +10495,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="375" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="0" t="s">
         <v>1433</v>
       </c>
@@ -10520,7 +10509,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="376" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="376" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="0" t="s">
         <v>1437</v>
       </c>
@@ -10534,7 +10523,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="377" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="377" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="0" t="s">
         <v>1441</v>
       </c>
@@ -10548,7 +10537,7 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="378" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="378" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="0" t="s">
         <v>1445</v>
       </c>
@@ -10562,7 +10551,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="379" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="379" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="0" t="s">
         <v>1449</v>
       </c>
@@ -10576,7 +10565,7 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="380" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="380" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="0" t="s">
         <v>1453</v>
       </c>
@@ -10590,7 +10579,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="381" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="0" t="s">
         <v>1457</v>
       </c>
@@ -10604,23 +10593,23 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="382" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="382" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="0" t="s">
+        <v>656</v>
+      </c>
+      <c r="B382" s="1" t="s">
         <v>1461</v>
       </c>
-      <c r="B382" s="1" t="s">
+      <c r="C382" s="1" t="s">
         <v>1462</v>
       </c>
-      <c r="C382" s="1" t="s">
+      <c r="D382" s="0" t="s">
         <v>1463</v>
       </c>
-      <c r="D382" s="0" t="s">
+    </row>
+    <row r="383" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="0" t="s">
         <v>1464</v>
-      </c>
-    </row>
-    <row r="383" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="0" t="s">
-        <v>660</v>
       </c>
       <c r="B383" s="1" t="s">
         <v>1465</v>
@@ -10632,7 +10621,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="384" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="0" t="s">
         <v>1468</v>
       </c>
@@ -10646,7 +10635,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="385" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="385" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="0" t="s">
         <v>1472</v>
       </c>
@@ -10660,7 +10649,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="386" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="386" customFormat="false" ht="372.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="0" t="s">
         <v>1476</v>
       </c>
@@ -10668,43 +10657,43 @@
         <v>1477</v>
       </c>
       <c r="C386" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D386" s="0" t="s">
         <v>1478</v>
       </c>
-      <c r="D386" s="0" t="s">
+    </row>
+    <row r="387" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="0" t="s">
         <v>1479</v>
       </c>
-    </row>
-    <row r="387" customFormat="false" ht="372.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="0" t="s">
+      <c r="B387" s="1" t="s">
         <v>1480</v>
       </c>
-      <c r="B387" s="1" t="s">
+      <c r="C387" s="1" t="s">
         <v>1481</v>
-      </c>
-      <c r="C387" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="D387" s="0" t="s">
         <v>1482</v>
       </c>
     </row>
-    <row r="388" customFormat="false" ht="406.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="B388" s="1" t="s">
         <v>1483</v>
       </c>
-      <c r="B388" s="1" t="s">
+      <c r="C388" s="1" t="s">
         <v>1484</v>
       </c>
-      <c r="C388" s="1" t="s">
+      <c r="D388" s="0" t="s">
         <v>1485</v>
       </c>
-      <c r="D388" s="0" t="s">
+    </row>
+    <row r="389" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="0" t="s">
         <v>1486</v>
-      </c>
-    </row>
-    <row r="389" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="0" t="s">
-        <v>378</v>
       </c>
       <c r="B389" s="1" t="s">
         <v>1487</v>
@@ -10716,37 +10705,37 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="390" customFormat="false" ht="586.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" customFormat="false" ht="350.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B390" s="1" t="s">
         <v>1490</v>
       </c>
-      <c r="B390" s="1" t="s">
+      <c r="C390" s="1" t="s">
         <v>1491</v>
       </c>
-      <c r="C390" s="1" t="s">
+      <c r="D390" s="0" t="s">
         <v>1492</v>
       </c>
-      <c r="D390" s="0" t="s">
+    </row>
+    <row r="391" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A391" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="B391" s="1" t="s">
         <v>1493</v>
       </c>
-    </row>
-    <row r="391" customFormat="false" ht="350.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B391" s="1" t="s">
+      <c r="C391" s="1" t="s">
         <v>1494</v>
       </c>
-      <c r="C391" s="1" t="s">
+      <c r="D391" s="0" t="s">
         <v>1495</v>
       </c>
-      <c r="D391" s="0" t="s">
+    </row>
+    <row r="392" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A392" s="0" t="s">
         <v>1496</v>
-      </c>
-    </row>
-    <row r="392" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="0" t="s">
-        <v>534</v>
       </c>
       <c r="B392" s="1" t="s">
         <v>1497</v>
@@ -10758,7 +10747,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="393" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="393" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="0" t="s">
         <v>1500</v>
       </c>
@@ -10772,7 +10761,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="394" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="394" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="0" t="s">
         <v>1504</v>
       </c>
@@ -10786,51 +10775,51 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="395" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B395" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C395" s="1" t="s">
         <v>1508</v>
       </c>
-      <c r="B395" s="1" t="s">
+      <c r="D395" s="0" t="s">
         <v>1509</v>
       </c>
-      <c r="C395" s="1" t="s">
+    </row>
+    <row r="396" customFormat="false" ht="665.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A396" s="0" t="s">
+        <v>538</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="D396" s="0" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A397" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B397" s="1" t="s">
         <v>1510</v>
       </c>
-      <c r="D395" s="0" t="s">
+      <c r="C397" s="1" t="s">
         <v>1511</v>
       </c>
-    </row>
-    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="B396" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C396" s="1" t="s">
+      <c r="D397" s="0" t="s">
         <v>1512</v>
       </c>
-      <c r="D396" s="0" t="s">
+    </row>
+    <row r="398" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A398" s="0" t="s">
         <v>1513</v>
-      </c>
-    </row>
-    <row r="397" customFormat="false" ht="665.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="B397" s="1" t="s">
-        <v>878</v>
-      </c>
-      <c r="C397" s="1" t="s">
-        <v>879</v>
-      </c>
-      <c r="D397" s="0" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="398" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="0" t="s">
-        <v>112</v>
       </c>
       <c r="B398" s="1" t="s">
         <v>1514</v>
@@ -10856,7 +10845,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="400" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="400" customFormat="false" ht="1869.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
         <v>1521</v>
       </c>
@@ -10870,7 +10859,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="401" customFormat="false" ht="1869.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="401" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="0" t="s">
         <v>1525</v>
       </c>
@@ -10884,37 +10873,37 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="402" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
+        <v>755</v>
+      </c>
+      <c r="B402" s="1" t="s">
         <v>1529</v>
       </c>
-      <c r="B402" s="1" t="s">
+      <c r="C402" s="1" t="s">
         <v>1530</v>
       </c>
-      <c r="C402" s="1" t="s">
+      <c r="D402" s="0" t="s">
         <v>1531</v>
       </c>
-      <c r="D402" s="0" t="s">
+    </row>
+    <row r="403" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="0" t="s">
+        <v>638</v>
+      </c>
+      <c r="B403" s="1" t="s">
         <v>1532</v>
       </c>
-    </row>
-    <row r="403" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="0" t="s">
-        <v>759</v>
-      </c>
-      <c r="B403" s="1" t="s">
+      <c r="C403" s="1" t="s">
         <v>1533</v>
       </c>
-      <c r="C403" s="1" t="s">
+      <c r="D403" s="0" t="s">
         <v>1534</v>
       </c>
-      <c r="D403" s="0" t="s">
+    </row>
+    <row r="404" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A404" s="0" t="s">
         <v>1535</v>
-      </c>
-    </row>
-    <row r="404" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="0" t="s">
-        <v>642</v>
       </c>
       <c r="B404" s="1" t="s">
         <v>1536</v>
@@ -10926,7 +10915,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="405" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="405" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="0" t="s">
         <v>1539</v>
       </c>
@@ -10940,7 +10929,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="406" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="406" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="0" t="s">
         <v>1543</v>
       </c>
@@ -10954,7 +10943,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="407" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="407" customFormat="false" ht="429" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
         <v>1547</v>
       </c>
@@ -10968,7 +10957,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="408" customFormat="false" ht="429" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="408" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
         <v>1551</v>
       </c>
@@ -10982,7 +10971,7 @@
         <v>1554</v>
       </c>
     </row>
-    <row r="409" customFormat="false" ht="102.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="409" customFormat="false" ht="631.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
         <v>1555</v>
       </c>
@@ -10996,7 +10985,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="410" customFormat="false" ht="631.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="410" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="0" t="s">
         <v>1559</v>
       </c>
@@ -11010,7 +10999,7 @@
         <v>1562</v>
       </c>
     </row>
-    <row r="411" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="411" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="0" t="s">
         <v>1563</v>
       </c>
@@ -11024,7 +11013,7 @@
         <v>1566</v>
       </c>
     </row>
-    <row r="412" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="412" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
         <v>1567</v>
       </c>
@@ -11038,7 +11027,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="413" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="413" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
         <v>1571</v>
       </c>
@@ -11052,7 +11041,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="414" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="414" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
         <v>1575</v>
       </c>
@@ -11066,7 +11055,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="415" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" customFormat="false" ht="744" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="0" t="s">
         <v>1579</v>
       </c>
@@ -11080,7 +11069,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="416" customFormat="false" ht="744" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="416" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="0" t="s">
         <v>1583</v>
       </c>
@@ -11094,7 +11083,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="417" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
         <v>1587</v>
       </c>
@@ -11108,7 +11097,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="418" customFormat="false" ht="822.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="s">
         <v>1591</v>
       </c>
@@ -11122,7 +11111,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="419" customFormat="false" ht="822.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="419" customFormat="false" ht="395.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
         <v>1595</v>
       </c>
@@ -11136,7 +11125,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="420" customFormat="false" ht="395.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="420" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="0" t="s">
         <v>1599</v>
       </c>
@@ -11150,35 +11139,35 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="421" customFormat="false" ht="294" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="421" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="B421" s="1" t="s">
         <v>1603</v>
       </c>
-      <c r="B421" s="1" t="s">
+      <c r="C421" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D421" s="0" t="s">
         <v>1604</v>
       </c>
-      <c r="C421" s="1" t="s">
+    </row>
+    <row r="422" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="0" t="s">
         <v>1605</v>
       </c>
-      <c r="D421" s="0" t="s">
+      <c r="B422" s="1" t="s">
         <v>1606</v>
       </c>
-    </row>
-    <row r="422" customFormat="false" ht="215.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="0" t="s">
-        <v>912</v>
-      </c>
-      <c r="B422" s="1" t="s">
+      <c r="C422" s="1" t="s">
         <v>1607</v>
-      </c>
-      <c r="C422" s="1" t="s">
-        <v>914</v>
       </c>
       <c r="D422" s="0" t="s">
         <v>1608</v>
       </c>
     </row>
-    <row r="423" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="423" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
         <v>1609</v>
       </c>
@@ -11192,7 +11181,7 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="424" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="424" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="0" t="s">
         <v>1613</v>
       </c>
@@ -11206,35 +11195,35 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="425" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="0" t="s">
-        <v>1617</v>
+        <v>668</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>1618</v>
+        <v>669</v>
       </c>
       <c r="C425" s="1" t="s">
-        <v>1619</v>
+        <v>670</v>
       </c>
       <c r="D425" s="0" t="s">
-        <v>1620</v>
+        <v>671</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>672</v>
+        <v>1617</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>673</v>
+        <v>1618</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>674</v>
+        <v>1619</v>
       </c>
       <c r="D426" s="0" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="427" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="2072.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
         <v>1621</v>
       </c>
@@ -11248,7 +11237,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="428" customFormat="false" ht="2072.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="428" customFormat="false" ht="3141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
         <v>1625</v>
       </c>
@@ -11262,7 +11251,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="429" customFormat="false" ht="3141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="0" t="s">
         <v>1629</v>
       </c>
@@ -11276,23 +11265,23 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="430" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B430" s="1" t="s">
         <v>1633</v>
       </c>
-      <c r="B430" s="1" t="s">
+      <c r="C430" s="1" t="s">
         <v>1634</v>
       </c>
-      <c r="C430" s="1" t="s">
+      <c r="D430" s="0" t="s">
         <v>1635</v>
       </c>
-      <c r="D430" s="0" t="s">
+    </row>
+    <row r="431" customFormat="false" ht="1228.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A431" s="0" t="s">
         <v>1636</v>
-      </c>
-    </row>
-    <row r="431" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="0" t="s">
-        <v>390</v>
       </c>
       <c r="B431" s="1" t="s">
         <v>1637</v>
@@ -11304,7 +11293,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="432" customFormat="false" ht="1228.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="432" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="0" t="s">
         <v>1640</v>
       </c>
@@ -11318,7 +11307,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="433" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
         <v>1644</v>
       </c>
@@ -11332,23 +11321,23 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="434" customFormat="false" ht="305.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
+        <v>692</v>
+      </c>
+      <c r="B434" s="1" t="s">
         <v>1648</v>
       </c>
-      <c r="B434" s="1" t="s">
+      <c r="C434" s="1" t="s">
         <v>1649</v>
       </c>
-      <c r="C434" s="1" t="s">
+      <c r="D434" s="0" t="s">
         <v>1650</v>
       </c>
-      <c r="D434" s="0" t="s">
+    </row>
+    <row r="435" customFormat="false" ht="1566" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="0" t="s">
         <v>1651</v>
-      </c>
-    </row>
-    <row r="435" customFormat="false" ht="305.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="0" t="s">
-        <v>696</v>
       </c>
       <c r="B435" s="1" t="s">
         <v>1652</v>
@@ -11360,7 +11349,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="436" customFormat="false" ht="1566" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="436" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
         <v>1655</v>
       </c>
@@ -11374,7 +11363,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="437" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="437" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="0" t="s">
         <v>1659</v>
       </c>
@@ -11402,7 +11391,7 @@
         <v>1666</v>
       </c>
     </row>
-    <row r="439" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="439" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
         <v>1667</v>
       </c>
@@ -11416,7 +11405,7 @@
         <v>1670</v>
       </c>
     </row>
-    <row r="440" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
         <v>1671</v>
       </c>
@@ -11430,7 +11419,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="441" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
         <v>1675</v>
       </c>
@@ -11444,35 +11433,35 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="442" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="442" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="0" t="s">
+        <v>743</v>
+      </c>
+      <c r="B442" s="1" t="s">
         <v>1679</v>
       </c>
-      <c r="B442" s="1" t="s">
+      <c r="C442" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="D442" s="0" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="552.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="0" t="s">
         <v>1680</v>
       </c>
-      <c r="C442" s="1" t="s">
+      <c r="B443" s="1" t="s">
         <v>1681</v>
       </c>
-      <c r="D442" s="0" t="s">
+      <c r="C443" s="1" t="s">
         <v>1682</v>
       </c>
-    </row>
-    <row r="443" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="0" t="s">
-        <v>747</v>
-      </c>
-      <c r="B443" s="1" t="s">
+      <c r="D443" s="0" t="s">
         <v>1683</v>
       </c>
-      <c r="C443" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="D443" s="0" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="444" customFormat="false" ht="552.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="444" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="0" t="s">
         <v>1684</v>
       </c>
@@ -11486,7 +11475,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="445" customFormat="false" ht="260.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="445" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="s">
         <v>1688</v>
       </c>
@@ -11500,7 +11489,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="446" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="446" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="0" t="s">
         <v>1692</v>
       </c>
@@ -11514,7 +11503,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="447" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="447" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="0" t="s">
         <v>1696</v>
       </c>
@@ -11528,7 +11517,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="448" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="448" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="0" t="s">
         <v>1700</v>
       </c>
@@ -11542,7 +11531,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="449" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="0" t="s">
         <v>1704</v>
       </c>
@@ -11554,20 +11543,6 @@
       </c>
       <c r="D449" s="0" t="s">
         <v>1707</v>
-      </c>
-    </row>
-    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="0" t="s">
-        <v>1708</v>
-      </c>
-      <c r="B450" s="1" t="s">
-        <v>1709</v>
-      </c>
-      <c r="C450" s="1" t="s">
-        <v>1710</v>
-      </c>
-      <c r="D450" s="0" t="s">
-        <v>1711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>